<commit_message>
feat: Add Profile module automation with comprehensive logging
- Implemented Profile module with 3 test cases (TC01-TC03)
  * Add Valid Billing Address
  * Add Shipping Address
  * Verify Address Persistence After Logout/Login

- Added comprehensive logging to all test modules
  * Login tests: detailed step-by-step logging
  * Registration tests: credential generation and validation logging
  * Profile tests: address operations and persistence logging
  * Cart tests: product operations logging

- Created profile_page.py with POM for address management
  * Billing and shipping address support
  * Field validation and state handling

- Enhanced test infrastructure
  * Added pytest.ini for log capture in HTML reports
  * Updated all test runners with sys.path configuration
  * Created comprehensive README.md with all test case documentation

- Test Results: 19/19 tests passing
  * Cart: 5/5 ✅
  * Login: 5/5 ✅
  * Profile: 3/3 ✅
  * Registration: 6/6 ✅
</commit_message>
<xml_diff>
--- a/testdata/Login Testcases.xlsx
+++ b/testdata/Login Testcases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\naveen.prakash\Downloads\automationpractice-site-automation\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F979B4A5-7912-492F-A44E-5EC61AF5F03C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1461730E-852A-4C1D-83FD-308246733D15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{09C35932-9D2A-460C-93CE-0190B5562E0E}"/>
   </bookViews>
@@ -83,9 +83,6 @@
     <t>Email: (empty) Password: (empty)</t>
   </si>
   <si>
-    <t>LOG-01</t>
-  </si>
-  <si>
     <t>Login</t>
   </si>
   <si>
@@ -107,9 +104,6 @@
     <t>Username (or user name) is displayed on page. Session starts.</t>
   </si>
   <si>
-    <t>LOG-02</t>
-  </si>
-  <si>
     <t>Login with email in different case</t>
   </si>
   <si>
@@ -125,9 +119,6 @@
     <t>Email should be case-insensitive.</t>
   </si>
   <si>
-    <t>LOG-NEG-01</t>
-  </si>
-  <si>
     <t>Login with incorrect password</t>
   </si>
   <si>
@@ -146,9 +137,6 @@
     <t>User is not logged in. Error message appears.</t>
   </si>
   <si>
-    <t>LOG-NEG-02</t>
-  </si>
-  <si>
     <t>Login with non-existent email</t>
   </si>
   <si>
@@ -167,9 +155,6 @@
     <t>Verify system rejects unregistered emails.</t>
   </si>
   <si>
-    <t>LOG-NEG-03</t>
-  </si>
-  <si>
     <t>Login with blank fields</t>
   </si>
   <si>
@@ -186,6 +171,21 @@
   </si>
   <si>
     <t>Email: User123@mail.com Password: Str0ngPass!</t>
+  </si>
+  <si>
+    <t>TC_Login_CorrectCredentials</t>
+  </si>
+  <si>
+    <t>TC_Login_EmailDifferentCase</t>
+  </si>
+  <si>
+    <t>NTC_Login_IncorrectPassword</t>
+  </si>
+  <si>
+    <t>NTC_Login_NonExistentEmail</t>
+  </si>
+  <si>
+    <t>NTC_Login_BlankFields</t>
   </si>
 </sst>
 </file>
@@ -605,8 +605,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3AE4E1E-5182-49F9-85E3-97AC96FBB8F6}">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -644,160 +644,160 @@
       </c>
     </row>
     <row r="2" spans="1:10" ht="90" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>18</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>21</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>22</v>
       </c>
       <c r="J2" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="100" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
-        <v>36</v>
+      <c r="A5" t="s">
+        <v>48</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>10</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="70" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
-        <v>43</v>
+      <c r="A6" t="s">
+        <v>49</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="H6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="J6" s="2" t="s">
         <v>11</v>

</xml_diff>